<commit_message>
update code and latest measurements
</commit_message>
<xml_diff>
--- a/measurements/container-measurements.xlsx
+++ b/measurements/container-measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhultonharrop/Documents/Projects/map-vector/measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A2A0C7-2992-F247-8A90-CC9FF9BC8A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C77101-F925-8042-80F3-B9B113295C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="680" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
+    <workbookView xWindow="920" yWindow="680" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="30">
   <si>
     <t>unordered_map</t>
   </si>
@@ -101,6 +101,30 @@
   </si>
   <si>
     <t>percenrage vs map</t>
+  </si>
+  <si>
+    <t>32 bytes</t>
+  </si>
+  <si>
+    <t>64 bytes</t>
+  </si>
+  <si>
+    <t>128 bytes</t>
+  </si>
+  <si>
+    <t>256 bytes</t>
+  </si>
+  <si>
+    <t>512 bytes</t>
+  </si>
+  <si>
+    <t>1024 bytes</t>
+  </si>
+  <si>
+    <t>2048 bytes</t>
+  </si>
+  <si>
+    <t>4096 bytes</t>
   </si>
 </sst>
 </file>
@@ -5041,37 +5065,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>23.2</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.6</c:v>
+                  <c:v>55.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>359</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1506</c:v>
+                  <c:v>1472</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3011</c:v>
+                  <c:v>2992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5956</c:v>
+                  <c:v>5967</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12957</c:v>
+                  <c:v>12789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26809</c:v>
+                  <c:v>27115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81774</c:v>
+                  <c:v>65110</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>828267</c:v>
+                  <c:v>826671</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1880164</c:v>
+                  <c:v>1944433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5173,37 +5197,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>10.7</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.1</c:v>
+                  <c:v>25.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.8</c:v>
+                  <c:v>58.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>164</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>659</c:v>
+                  <c:v>638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1290</c:v>
+                  <c:v>1288</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3329</c:v>
+                  <c:v>2921</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16169</c:v>
+                  <c:v>16376</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37443</c:v>
+                  <c:v>37244</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>79058</c:v>
+                  <c:v>79909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5570,37 +5594,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>23.3</c:v>
+                  <c:v>23.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.3</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1556</c:v>
+                  <c:v>1552</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3090</c:v>
+                  <c:v>3115</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6677</c:v>
+                  <c:v>6821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14209</c:v>
+                  <c:v>14147</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30734</c:v>
+                  <c:v>31181</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104939</c:v>
+                  <c:v>94594</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>873321</c:v>
+                  <c:v>867609</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1997212</c:v>
+                  <c:v>1986803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5699,37 +5723,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>10.8</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.5</c:v>
+                  <c:v>28.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>106</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>222</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>319</c:v>
+                  <c:v>461</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>915</c:v>
+                  <c:v>936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1889</c:v>
+                  <c:v>2133</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11285</c:v>
+                  <c:v>11309</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24459</c:v>
+                  <c:v>24323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50794</c:v>
+                  <c:v>52095</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>97684</c:v>
+                  <c:v>100717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5873,6 +5897,1318 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="768715327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$C$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$C$117:$C$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.8918918918918919</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0381679389312977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7494908350305498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9550561797752808</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0833333333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1371951219512195</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6944444444444446</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.6526806526806528</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3734707018673529</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.600156188988676</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.753674309229865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$D$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$D$117:$D$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.9811320754716981</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9925093632958804</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8033472803347284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9471316085489314</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0773809523809526</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1615853658536586</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.202143950995406</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0168516235100702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1816394731668964</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.1375858684985278</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8023952095808387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$E$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$E$117:$E$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.9811320754716981</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8896797153024911</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7291242362525456</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8822882288228819</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.059171597633136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.621212121212121</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3993506493506498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1614296936370776</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.8982785602503913</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3135527589545015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.8099800593356354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$F$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$F$117:$F$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.9811320754716981</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9345454545454546</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7235772357723578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9208472686733558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9712643678160919</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1717011128775834</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8609375000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8573661586557257</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9458292443572134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.190563666247703</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.560492222718596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$G$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$G$117:$G$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9275362318840579</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8092243186582806</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9438202247191012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6206896551724137</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9122257053291536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.882215288611544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.6702002355712597</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.015118790496761</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.9742177522349937</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7449462150731012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$H$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$H$117:$H$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.1574074074074074</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1064638783269962</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7657841140529529</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6624203821656049</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6320754716981138</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6446540880503147</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7413522012578611</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.003106796116505</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.029548472775565</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.595290916082469</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.298997179144564</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$I$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$I$117:$I$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.1698113207547172</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1640625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6243567753001718</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3793103448275854</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.352664576802507</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.929347826086957</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2827798699075661</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9759404005862238</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.196085275480613</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.333091391457785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$J$116</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4096 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$117:$B$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$J$117:$J$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.1792452830188682</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9097222222222221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7589285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5485232067510548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.75704989154013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2873931623931627</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6324425691514302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7571845432841098</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8890761830366318</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.65436222286208</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.7265903472105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D802-6E49-8417-6BB50684A2FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="270830191"/>
+        <c:axId val="802783919"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="270830191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802783919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="802783919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="270830191"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11910,6 +13246,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -16875,6 +18251,522 @@
 </file>
 
 <file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22173,6 +24065,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A484C107-BB8E-7B43-85B9-1AC7BA4A748E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -22475,8 +24403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD4748D-2C7E-9A48-826D-471EC314D44C}">
   <dimension ref="C3:M126"/>
   <sheetViews>
-    <sheetView topLeftCell="G96" workbookViewId="0">
-      <selection activeCell="I134" sqref="I134"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="L116" sqref="L116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25849,10 +27777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37D38E-5F04-4043-B2C6-9B4BB7553281}">
-  <dimension ref="B3:E113"/>
+  <dimension ref="B3:J127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89:C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26990,14 +28918,14 @@
         <v>32</v>
       </c>
       <c r="C89">
-        <v>23.2</v>
+        <v>23</v>
       </c>
       <c r="D89">
-        <v>10.7</v>
+        <v>10.6</v>
       </c>
       <c r="E89">
         <f>C89/D89</f>
-        <v>2.1682242990654208</v>
+        <v>2.1698113207547172</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.2">
@@ -27005,14 +28933,14 @@
         <v>64</v>
       </c>
       <c r="C90">
-        <v>55.6</v>
+        <v>55.4</v>
       </c>
       <c r="D90">
-        <v>26.1</v>
+        <v>25.6</v>
       </c>
       <c r="E90">
         <f t="shared" ref="E90:E99" si="6">C90/D90</f>
-        <v>2.1302681992337162</v>
+        <v>2.1640625</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.2">
@@ -27020,14 +28948,14 @@
         <v>128</v>
       </c>
       <c r="C91">
-        <v>359</v>
+        <v>153</v>
       </c>
       <c r="D91">
-        <v>60.8</v>
+        <v>58.3</v>
       </c>
       <c r="E91">
         <f t="shared" si="6"/>
-        <v>5.9046052631578947</v>
+        <v>2.6243567753001718</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.2">
@@ -27035,14 +28963,14 @@
         <v>256</v>
       </c>
       <c r="C92">
-        <v>1506</v>
+        <v>1472</v>
       </c>
       <c r="D92">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E92">
         <f t="shared" si="6"/>
-        <v>9.1829268292682933</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.2">
@@ -27050,14 +28978,14 @@
         <v>512</v>
       </c>
       <c r="C93">
-        <v>3011</v>
+        <v>2992</v>
       </c>
       <c r="D93">
         <v>319</v>
       </c>
       <c r="E93">
         <f t="shared" si="6"/>
-        <v>9.4388714733542312</v>
+        <v>9.3793103448275854</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.2">
@@ -27065,14 +28993,14 @@
         <v>1024</v>
       </c>
       <c r="C94">
-        <v>5956</v>
+        <v>5967</v>
       </c>
       <c r="D94">
-        <v>659</v>
+        <v>638</v>
       </c>
       <c r="E94">
         <f t="shared" si="6"/>
-        <v>9.0379362670713199</v>
+        <v>9.352664576802507</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
@@ -27080,14 +29008,14 @@
         <v>2048</v>
       </c>
       <c r="C95">
-        <v>12957</v>
+        <v>12789</v>
       </c>
       <c r="D95">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E95">
         <f t="shared" si="6"/>
-        <v>10.044186046511628</v>
+        <v>9.929347826086957</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
@@ -27095,14 +29023,14 @@
         <v>4096</v>
       </c>
       <c r="C96">
-        <v>26809</v>
+        <v>27115</v>
       </c>
       <c r="D96">
-        <v>3329</v>
+        <v>2921</v>
       </c>
       <c r="E96">
         <f t="shared" si="6"/>
-        <v>8.0531691198558129</v>
+        <v>9.2827798699075661</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.2">
@@ -27110,14 +29038,14 @@
         <v>8192</v>
       </c>
       <c r="C97">
-        <v>81774</v>
+        <v>65110</v>
       </c>
       <c r="D97">
-        <v>16169</v>
+        <v>16376</v>
       </c>
       <c r="E97">
         <f t="shared" si="6"/>
-        <v>5.0574556249613458</v>
+        <v>3.9759404005862238</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.2">
@@ -27125,14 +29053,14 @@
         <v>16384</v>
       </c>
       <c r="C98">
-        <v>828267</v>
+        <v>826671</v>
       </c>
       <c r="D98">
-        <v>37443</v>
+        <v>37244</v>
       </c>
       <c r="E98">
         <f t="shared" si="6"/>
-        <v>22.120743530165853</v>
+        <v>22.196085275480613</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.2">
@@ -27140,14 +29068,14 @@
         <v>32768</v>
       </c>
       <c r="C99">
-        <v>1880164</v>
+        <v>1944433</v>
       </c>
       <c r="D99">
-        <v>79058</v>
+        <v>79909</v>
       </c>
       <c r="E99">
         <f t="shared" si="6"/>
-        <v>23.782084039565888</v>
+        <v>24.333091391457785</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.2">
@@ -27174,14 +29102,14 @@
         <v>32</v>
       </c>
       <c r="C103">
-        <v>23.3</v>
+        <v>23.1</v>
       </c>
       <c r="D103">
-        <v>10.8</v>
+        <v>10.6</v>
       </c>
       <c r="E103">
         <f>C103/D103</f>
-        <v>2.1574074074074074</v>
+        <v>2.1792452830188682</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.2">
@@ -27189,14 +29117,14 @@
         <v>64</v>
       </c>
       <c r="C104">
-        <v>55.3</v>
+        <v>55</v>
       </c>
       <c r="D104">
-        <v>27.5</v>
+        <v>28.8</v>
       </c>
       <c r="E104">
         <f t="shared" ref="E104:E113" si="7">C104/D104</f>
-        <v>2.0109090909090908</v>
+        <v>1.9097222222222221</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.2">
@@ -27204,14 +29132,14 @@
         <v>128</v>
       </c>
       <c r="C105">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="D105">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E105">
         <f t="shared" si="7"/>
-        <v>1.4245283018867925</v>
+        <v>1.7589285714285714</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.2">
@@ -27219,14 +29147,14 @@
         <v>256</v>
       </c>
       <c r="C106">
-        <v>1556</v>
+        <v>1552</v>
       </c>
       <c r="D106">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="E106">
         <f t="shared" si="7"/>
-        <v>7.0090090090090094</v>
+        <v>6.5485232067510548</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.2">
@@ -27234,14 +29162,14 @@
         <v>512</v>
       </c>
       <c r="C107">
-        <v>3090</v>
+        <v>3115</v>
       </c>
       <c r="D107">
-        <v>319</v>
+        <v>461</v>
       </c>
       <c r="E107">
         <f t="shared" si="7"/>
-        <v>9.6865203761755492</v>
+        <v>6.75704989154013</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.2">
@@ -27249,14 +29177,14 @@
         <v>1024</v>
       </c>
       <c r="C108">
-        <v>6677</v>
+        <v>6821</v>
       </c>
       <c r="D108">
-        <v>915</v>
+        <v>936</v>
       </c>
       <c r="E108">
         <f t="shared" si="7"/>
-        <v>7.2972677595628417</v>
+        <v>7.2873931623931627</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.2">
@@ -27264,14 +29192,14 @@
         <v>2048</v>
       </c>
       <c r="C109">
-        <v>14209</v>
+        <v>14147</v>
       </c>
       <c r="D109">
-        <v>1889</v>
+        <v>2133</v>
       </c>
       <c r="E109">
         <f t="shared" si="7"/>
-        <v>7.5219692959237694</v>
+        <v>6.6324425691514302</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.2">
@@ -27279,14 +29207,14 @@
         <v>4096</v>
       </c>
       <c r="C110">
-        <v>30734</v>
+        <v>31181</v>
       </c>
       <c r="D110">
-        <v>11285</v>
+        <v>11309</v>
       </c>
       <c r="E110">
         <f t="shared" si="7"/>
-        <v>2.7234381922906512</v>
+        <v>2.7571845432841098</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.2">
@@ -27294,14 +29222,14 @@
         <v>8192</v>
       </c>
       <c r="C111">
-        <v>104939</v>
+        <v>94594</v>
       </c>
       <c r="D111">
-        <v>24459</v>
+        <v>24323</v>
       </c>
       <c r="E111">
         <f t="shared" si="7"/>
-        <v>4.2904043501369635</v>
+        <v>3.8890761830366318</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.2">
@@ -27309,29 +29237,465 @@
         <v>16384</v>
       </c>
       <c r="C112">
-        <v>873321</v>
+        <v>867609</v>
       </c>
       <c r="D112">
-        <v>50794</v>
+        <v>52095</v>
       </c>
       <c r="E112">
         <f t="shared" si="7"/>
-        <v>17.193388982950744</v>
+        <v>16.65436222286208</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B113" s="1">
         <v>32768</v>
       </c>
       <c r="C113">
-        <v>1997212</v>
+        <v>1986803</v>
       </c>
       <c r="D113">
-        <v>97684</v>
+        <v>100717</v>
       </c>
       <c r="E113">
         <f t="shared" si="7"/>
-        <v>20.445641046640187</v>
+        <v>19.7265903472105</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s">
+        <v>22</v>
+      </c>
+      <c r="D116" t="s">
+        <v>23</v>
+      </c>
+      <c r="E116" t="s">
+        <v>24</v>
+      </c>
+      <c r="F116" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" t="s">
+        <v>26</v>
+      </c>
+      <c r="H116" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" t="s">
+        <v>28</v>
+      </c>
+      <c r="J116" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>32</v>
+      </c>
+      <c r="C117">
+        <f>E5</f>
+        <v>1.8918918918918919</v>
+      </c>
+      <c r="D117">
+        <f>E19</f>
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="E117">
+        <f>E33</f>
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="F117">
+        <f>E47</f>
+        <v>1.9811320754716981</v>
+      </c>
+      <c r="G117">
+        <f>E61</f>
+        <v>2</v>
+      </c>
+      <c r="H117">
+        <f>E75</f>
+        <v>2.1574074074074074</v>
+      </c>
+      <c r="I117">
+        <f>E89</f>
+        <v>2.1698113207547172</v>
+      </c>
+      <c r="J117">
+        <f>E103</f>
+        <v>2.1792452830188682</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>64</v>
+      </c>
+      <c r="C118">
+        <f t="shared" ref="C118:C127" si="8">E6</f>
+        <v>2.0381679389312977</v>
+      </c>
+      <c r="D118">
+        <f t="shared" ref="D118:D127" si="9">E20</f>
+        <v>1.9925093632958804</v>
+      </c>
+      <c r="E118">
+        <f t="shared" ref="E118:E127" si="10">E34</f>
+        <v>1.8896797153024911</v>
+      </c>
+      <c r="F118">
+        <f t="shared" ref="F118:F127" si="11">E48</f>
+        <v>1.9345454545454546</v>
+      </c>
+      <c r="G118">
+        <f t="shared" ref="G118:G127" si="12">E62</f>
+        <v>1.9275362318840579</v>
+      </c>
+      <c r="H118">
+        <f t="shared" ref="H118:H127" si="13">E76</f>
+        <v>2.1064638783269962</v>
+      </c>
+      <c r="I118">
+        <f t="shared" ref="I118:I127" si="14">E90</f>
+        <v>2.1640625</v>
+      </c>
+      <c r="J118">
+        <f t="shared" ref="J118:J127" si="15">E104</f>
+        <v>1.9097222222222221</v>
+      </c>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>128</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="8"/>
+        <v>2.7494908350305498</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="9"/>
+        <v>2.8033472803347284</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="10"/>
+        <v>2.7291242362525456</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="11"/>
+        <v>2.7235772357723578</v>
+      </c>
+      <c r="G119">
+        <f t="shared" si="12"/>
+        <v>2.8092243186582806</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="13"/>
+        <v>4.7657841140529529</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="14"/>
+        <v>2.6243567753001718</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="15"/>
+        <v>1.7589285714285714</v>
+      </c>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>256</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="8"/>
+        <v>2.9550561797752808</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="9"/>
+        <v>2.9471316085489314</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="10"/>
+        <v>2.8822882288228819</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="11"/>
+        <v>2.9208472686733558</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="12"/>
+        <v>2.9438202247191012</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="13"/>
+        <v>9.6624203821656049</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="14"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="15"/>
+        <v>6.5485232067510548</v>
+      </c>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>512</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="8"/>
+        <v>3.0833333333333335</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="9"/>
+        <v>3.0773809523809526</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="10"/>
+        <v>3.059171597633136</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="11"/>
+        <v>2.9712643678160919</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="12"/>
+        <v>1.6206896551724137</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="13"/>
+        <v>9.6320754716981138</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="14"/>
+        <v>9.3793103448275854</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="15"/>
+        <v>6.75704989154013</v>
+      </c>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>1024</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="8"/>
+        <v>3.1371951219512195</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="9"/>
+        <v>3.1615853658536586</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="10"/>
+        <v>12.621212121212121</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="11"/>
+        <v>9.1717011128775834</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="12"/>
+        <v>2.9122257053291536</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="13"/>
+        <v>9.6446540880503147</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="14"/>
+        <v>9.352664576802507</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="15"/>
+        <v>7.2873931623931627</v>
+      </c>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>2048</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="8"/>
+        <v>8.6944444444444446</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="9"/>
+        <v>11.202143950995406</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="10"/>
+        <v>6.3993506493506498</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="11"/>
+        <v>9.8609375000000004</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="12"/>
+        <v>9.882215288611544</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="13"/>
+        <v>9.7413522012578611</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="14"/>
+        <v>9.929347826086957</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="15"/>
+        <v>6.6324425691514302</v>
+      </c>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>4096</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="8"/>
+        <v>9.6526806526806528</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="9"/>
+        <v>6.0168516235100702</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="10"/>
+        <v>7.1614296936370776</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="11"/>
+        <v>9.8573661586557257</v>
+      </c>
+      <c r="G124">
+        <f t="shared" si="12"/>
+        <v>9.6702002355712597</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="13"/>
+        <v>10.003106796116505</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="14"/>
+        <v>9.2827798699075661</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="15"/>
+        <v>2.7571845432841098</v>
+      </c>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>8192</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="8"/>
+        <v>9.3734707018673529</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="9"/>
+        <v>6.1816394731668964</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="10"/>
+        <v>6.8982785602503913</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="11"/>
+        <v>9.9458292443572134</v>
+      </c>
+      <c r="G125">
+        <f t="shared" si="12"/>
+        <v>10.015118790496761</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="13"/>
+        <v>12.029548472775565</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="14"/>
+        <v>3.9759404005862238</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="15"/>
+        <v>3.8890761830366318</v>
+      </c>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B126" s="1">
+        <v>16384</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="8"/>
+        <v>11.600156188988676</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="9"/>
+        <v>6.1375858684985278</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="10"/>
+        <v>7.3135527589545015</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="11"/>
+        <v>10.190563666247703</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="12"/>
+        <v>8.9742177522349937</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="13"/>
+        <v>23.595290916082469</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="14"/>
+        <v>22.196085275480613</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="15"/>
+        <v>16.65436222286208</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B127" s="1">
+        <v>32768</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="8"/>
+        <v>10.753674309229865</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="9"/>
+        <v>6.8023952095808387</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="10"/>
+        <v>7.8099800593356354</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="11"/>
+        <v>14.560492222718596</v>
+      </c>
+      <c r="G127">
+        <f t="shared" si="12"/>
+        <v>6.7449462150731012</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="13"/>
+        <v>24.298997179144564</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="14"/>
+        <v>24.333091391457785</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="15"/>
+        <v>19.7265903472105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to compare handle iteration vs value iteration removal
</commit_message>
<xml_diff>
--- a/measurements/container-measurements.xlsx
+++ b/measurements/container-measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhultonharrop/Documents/Projects/map-vector/measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC09DC7-19C2-AB44-A303-964F15AAE267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E655C28-227F-764A-B072-7AC50CBB62B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="680" windowWidth="28040" windowHeight="17420" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="40">
   <si>
     <t>unordered_map</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>lookup-reverse-pointer</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -2939,6 +2942,569 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>element removal</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$F$148</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$E$149:$E$160</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$F$149:$F$160</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1756</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7748</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15508</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F52E-094F-A1E8-EE1FDFB9DE36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$G$148</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>handle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$E$149:$E$160</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$G$149:$G$160</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8171</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16858</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35970</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72838</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>161281</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F52E-094F-A1E8-EE1FDFB9DE36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="588332111"/>
+        <c:axId val="594499615"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="588332111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594499615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="594499615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588332111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3597,7 +4163,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -4270,7 +4836,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -4943,7 +5509,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -5625,7 +6191,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -6307,7 +6873,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -6988,7 +7554,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -7670,7 +8236,1049 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$D$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$C$20:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$D$20:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2097152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC09-7F46-AEE3-55FA811BDCAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>unordered_map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$C$20:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$E$20:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28672</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114688</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>229376</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>458752</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>917504</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1835008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3670016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EC09-7F46-AEE3-55FA811BDCAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$F$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>handle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$C$20:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$F$20:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2688</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5376</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10752</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21504</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>172032</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>344064</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>688128</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1376256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2752512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EC09-7F46-AEE3-55FA811BDCAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$G$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lookup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$C$20:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$G$20:$G$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4480</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17920</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35840</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71680</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>143360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>286720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>573440</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1146880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2293760</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4587520</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-EC09-7F46-AEE3-55FA811BDCAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$H$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lookup-reverse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$C$20:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$H$20:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6784</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54360</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>108864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>217896</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436032</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>872424</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1745296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3491128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6982816</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-20B5-5F41-989E-3F0335B7D6AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Memory!$I$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lookup-reverse-pointer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Memory!$C$20:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Memory!$I$20:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6272</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100672</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>201512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>403264</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>806888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1614224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3228984</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6458528</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-20B5-5F41-989E-3F0335B7D6AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1039845280"/>
+        <c:axId val="2008949408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1039845280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2008949408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2008949408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1039845280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -8453,1049 +10061,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Memory!$D$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>vector</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Memory!$C$20:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Memory!$D$20:$D$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>524288</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1048576</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2097152</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EC09-7F46-AEE3-55FA811BDCAD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Memory!$E$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>unordered_map</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Memory!$C$20:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Memory!$E$20:$E$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3584</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7168</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>28672</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>57344</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>114688</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>229376</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>458752</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>917504</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1835008</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3670016</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EC09-7F46-AEE3-55FA811BDCAD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Memory!$F$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>handle</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Memory!$C$20:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Memory!$F$20:$F$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2688</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5376</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10752</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21504</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43008</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>86016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>172032</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>344064</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>688128</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1376256</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2752512</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-EC09-7F46-AEE3-55FA811BDCAD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Memory!$G$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>lookup</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Memory!$C$20:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Memory!$G$20:$G$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4480</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8960</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17920</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35840</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>71680</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>143360</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>286720</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>573440</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1146880</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2293760</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4587520</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-EC09-7F46-AEE3-55FA811BDCAD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Memory!$H$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>lookup-reverse</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Memory!$C$20:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Memory!$H$20:$H$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6784</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13512</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27120</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54360</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108864</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>217896</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>436032</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>872424</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1745296</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3491128</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6982816</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-20B5-5F41-989E-3F0335B7D6AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Memory!$I$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>lookup-reverse-pointer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Memory!$C$20:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Memory!$I$20:$I$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>6272</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12488</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>25072</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50264</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100672</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>201512</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>403264</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>806888</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1614224</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3228984</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6458528</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-20B5-5F41-989E-3F0335B7D6AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1039845280"/>
-        <c:axId val="2008949408"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1039845280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2008949408"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2008949408"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1039845280"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -10965,7 +11531,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -11503,7 +12069,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -12041,7 +12607,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -19510,6 +20076,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -27531,6 +28137,522 @@
 </file>
 
 <file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -32051,6 +33173,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3BC4256-6D3C-8547-8329-F4DEBD306057}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -32793,9 +33951,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD4748D-2C7E-9A48-826D-471EC314D44C}">
-  <dimension ref="C3:O126"/>
+  <dimension ref="C3:O160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="K144" sqref="K144"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -36735,6 +37895,149 @@
       <c r="F126" s="2">
         <f>O106</f>
         <v>6.7114093959731542E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E148" t="s">
+        <v>2</v>
+      </c>
+      <c r="F148" t="s">
+        <v>39</v>
+      </c>
+      <c r="G148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E149">
+        <v>32</v>
+      </c>
+      <c r="F149">
+        <v>6.04</v>
+      </c>
+      <c r="G149">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="150" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E150">
+        <v>64</v>
+      </c>
+      <c r="F150">
+        <v>11</v>
+      </c>
+      <c r="G150">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="151" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E151">
+        <v>128</v>
+      </c>
+      <c r="F151">
+        <v>21.1</v>
+      </c>
+      <c r="G151">
+        <v>70.599999999999994</v>
+      </c>
+    </row>
+    <row r="152" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E152">
+        <v>256</v>
+      </c>
+      <c r="F152">
+        <v>53.4</v>
+      </c>
+      <c r="G152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E153">
+        <v>512</v>
+      </c>
+      <c r="F153">
+        <v>91.1</v>
+      </c>
+      <c r="G153">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="154" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E154">
+        <v>1024</v>
+      </c>
+      <c r="F154">
+        <v>172</v>
+      </c>
+      <c r="G154">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="155" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E155">
+        <v>2048</v>
+      </c>
+      <c r="F155">
+        <v>335</v>
+      </c>
+      <c r="G155">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="156" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E156">
+        <v>4096</v>
+      </c>
+      <c r="F156">
+        <v>655</v>
+      </c>
+      <c r="G156">
+        <v>8171</v>
+      </c>
+    </row>
+    <row r="157" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E157">
+        <v>8192</v>
+      </c>
+      <c r="F157">
+        <v>1756</v>
+      </c>
+      <c r="G157">
+        <v>16858</v>
+      </c>
+    </row>
+    <row r="158" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E158" s="1">
+        <v>16384</v>
+      </c>
+      <c r="F158">
+        <v>3882</v>
+      </c>
+      <c r="G158">
+        <v>35970</v>
+      </c>
+    </row>
+    <row r="159" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E159" s="1">
+        <v>32768</v>
+      </c>
+      <c r="F159">
+        <v>7748</v>
+      </c>
+      <c r="G159">
+        <v>72838</v>
+      </c>
+    </row>
+    <row r="160" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E160" s="1">
+        <v>65536</v>
+      </c>
+      <c r="F160">
+        <v>15508</v>
+      </c>
+      <c r="G160">
+        <v>161281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 'add' benchmarks and update measurements
</commit_message>
<xml_diff>
--- a/measurements/container-measurements.xlsx
+++ b/measurements/container-measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhultonharrop/Documents/Projects/map-vector/measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E0407D-A929-5B42-93CE-23D4883EBCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE0EF9E-E68F-314D-B39C-E4DE1D630C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="680" windowWidth="28040" windowHeight="17420" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
+    <workbookView xWindow="920" yWindow="680" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="51">
   <si>
     <t>unordered_map</t>
   </si>
@@ -170,6 +170,24 @@
   </si>
   <si>
     <t>unordered_map/packed-hashtable-rl % diff</t>
+  </si>
+  <si>
+    <t>packed-hashtable remove values</t>
+  </si>
+  <si>
+    <t>packed-hashtable-rl remove values</t>
+  </si>
+  <si>
+    <t>packed-hashtable-rl add values</t>
+  </si>
+  <si>
+    <t>unordered-map remove values</t>
+  </si>
+  <si>
+    <t>unordered-map add values</t>
+  </si>
+  <si>
+    <t>packed-hashtable add values</t>
   </si>
 </sst>
 </file>
@@ -13189,6 +13207,1412 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1201023680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>remove</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$V$162</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>packed-hashtable-rl remove values</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$U$163:$U$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$V$163:$V$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1739</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3832</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7679</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15652</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FFE9-6C48-8E6E-D73A947C4F8C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$W$162</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>packed-hashtable remove values</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$U$163:$U$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$W$163:$W$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7386</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17420</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36329</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72027</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>163285</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FFE9-6C48-8E6E-D73A947C4F8C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$X$162</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>unordered-map remove values</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$U$163:$U$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$X$163:$X$174</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7666</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20096</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40786</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79059</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>171665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FFE9-6C48-8E6E-D73A947C4F8C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="556607119"/>
+        <c:axId val="623065647"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="556607119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="623065647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="623065647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556607119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>add</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$V$176</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>packed-hashtable-rl add values</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$U$177:$U$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$V$177:$V$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2871</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5743</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11469</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22922</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45833</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91785</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>184051</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F44D-0746-B9DB-AE75FACDD8E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$W$176</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>packed-hashtable add values</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$U$177:$U$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$W$177:$W$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>88.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5090</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10187</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20379</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40716</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>81612</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>163207</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F44D-0746-B9DB-AE75FACDD8E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Performance!$X$176</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>unordered-map add values</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$U$177:$U$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$X$177:$X$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>40.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1278</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2898</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10712</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21090</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42211</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>86042</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F44D-0746-B9DB-AE75FACDD8E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1044816399"/>
+        <c:axId val="1045221119"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1044816399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1045221119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1045221119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044816399"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20670,6 +22094,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors25.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors26.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -29207,6 +30711,1038 @@
 </file>
 
 <file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style25.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style26.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -34171,16 +36707,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
       <xdr:row>159</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>172</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -34200,6 +36736,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78B293D2-FD56-5840-BE71-C320E3A98204}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52759DCC-9383-3D49-926F-287C20A59CE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -34507,8 +37115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD4748D-2C7E-9A48-826D-471EC314D44C}">
   <dimension ref="C3:S166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="M138" sqref="M138"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40558,10 +43166,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37D38E-5F04-4043-B2C6-9B4BB7553281}">
-  <dimension ref="B3:V158"/>
+  <dimension ref="B3:X188"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="U165" sqref="U165"/>
+    <sheetView tabSelected="1" topLeftCell="C140" workbookViewId="0">
+      <selection activeCell="AF181" sqref="AF181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40573,9 +43181,13 @@
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="34" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -43365,6 +45977,370 @@
       </c>
       <c r="V158">
         <v>337634</v>
+      </c>
+    </row>
+    <row r="162" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U162" t="s">
+        <v>2</v>
+      </c>
+      <c r="V162" t="s">
+        <v>46</v>
+      </c>
+      <c r="W162" t="s">
+        <v>45</v>
+      </c>
+      <c r="X162" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="163" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U163">
+        <v>32</v>
+      </c>
+      <c r="V163">
+        <v>5.9</v>
+      </c>
+      <c r="W163">
+        <v>16.7</v>
+      </c>
+      <c r="X163">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="164" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U164">
+        <v>64</v>
+      </c>
+      <c r="V164">
+        <v>10.9</v>
+      </c>
+      <c r="W164">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="X164">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="165" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U165">
+        <v>128</v>
+      </c>
+      <c r="V165">
+        <v>21</v>
+      </c>
+      <c r="W165">
+        <v>70.2</v>
+      </c>
+      <c r="X165">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="166" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U166">
+        <v>256</v>
+      </c>
+      <c r="V166">
+        <v>53.3</v>
+      </c>
+      <c r="W166">
+        <v>150</v>
+      </c>
+      <c r="X166">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="167" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U167">
+        <v>512</v>
+      </c>
+      <c r="V167">
+        <v>90.8</v>
+      </c>
+      <c r="W167">
+        <v>289</v>
+      </c>
+      <c r="X167">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="168" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U168">
+        <v>1024</v>
+      </c>
+      <c r="V168">
+        <v>171</v>
+      </c>
+      <c r="W168">
+        <v>573</v>
+      </c>
+      <c r="X168">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="169" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U169">
+        <v>2048</v>
+      </c>
+      <c r="V169">
+        <v>331</v>
+      </c>
+      <c r="W169">
+        <v>4304</v>
+      </c>
+      <c r="X169">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="170" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U170">
+        <v>4096</v>
+      </c>
+      <c r="V170">
+        <v>648</v>
+      </c>
+      <c r="W170">
+        <v>7386</v>
+      </c>
+      <c r="X170">
+        <v>7666</v>
+      </c>
+    </row>
+    <row r="171" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U171">
+        <v>8192</v>
+      </c>
+      <c r="V171">
+        <v>1739</v>
+      </c>
+      <c r="W171">
+        <v>17420</v>
+      </c>
+      <c r="X171">
+        <v>20096</v>
+      </c>
+    </row>
+    <row r="172" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U172" s="1">
+        <v>16384</v>
+      </c>
+      <c r="V172">
+        <v>3832</v>
+      </c>
+      <c r="W172">
+        <v>36329</v>
+      </c>
+      <c r="X172">
+        <v>40786</v>
+      </c>
+    </row>
+    <row r="173" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U173" s="1">
+        <v>32768</v>
+      </c>
+      <c r="V173">
+        <v>7679</v>
+      </c>
+      <c r="W173">
+        <v>72027</v>
+      </c>
+      <c r="X173">
+        <v>79059</v>
+      </c>
+    </row>
+    <row r="174" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U174" s="1">
+        <v>65536</v>
+      </c>
+      <c r="V174">
+        <v>15652</v>
+      </c>
+      <c r="W174">
+        <v>163285</v>
+      </c>
+      <c r="X174">
+        <v>171665</v>
+      </c>
+    </row>
+    <row r="176" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U176" t="s">
+        <v>2</v>
+      </c>
+      <c r="V176" t="s">
+        <v>47</v>
+      </c>
+      <c r="W176" t="s">
+        <v>50</v>
+      </c>
+      <c r="X176" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="177" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U177">
+        <v>32</v>
+      </c>
+      <c r="V177">
+        <v>96</v>
+      </c>
+      <c r="W177">
+        <v>88.1</v>
+      </c>
+      <c r="X177">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="178" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U178">
+        <v>64</v>
+      </c>
+      <c r="V178">
+        <v>186</v>
+      </c>
+      <c r="W178">
+        <v>167</v>
+      </c>
+      <c r="X178">
+        <v>86.3</v>
+      </c>
+    </row>
+    <row r="179" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U179">
+        <v>128</v>
+      </c>
+      <c r="V179">
+        <v>365</v>
+      </c>
+      <c r="W179">
+        <v>325</v>
+      </c>
+      <c r="X179">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="180" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U180">
+        <v>256</v>
+      </c>
+      <c r="V180">
+        <v>722</v>
+      </c>
+      <c r="W180">
+        <v>643</v>
+      </c>
+      <c r="X180">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="181" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U181">
+        <v>512</v>
+      </c>
+      <c r="V181">
+        <v>1440</v>
+      </c>
+      <c r="W181">
+        <v>1279</v>
+      </c>
+      <c r="X181">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="182" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U182">
+        <v>1024</v>
+      </c>
+      <c r="V182">
+        <v>2871</v>
+      </c>
+      <c r="W182">
+        <v>2551</v>
+      </c>
+      <c r="X182">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="183" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U183">
+        <v>2048</v>
+      </c>
+      <c r="V183">
+        <v>5743</v>
+      </c>
+      <c r="W183">
+        <v>5090</v>
+      </c>
+      <c r="X183">
+        <v>2898</v>
+      </c>
+    </row>
+    <row r="184" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U184">
+        <v>4096</v>
+      </c>
+      <c r="V184">
+        <v>11469</v>
+      </c>
+      <c r="W184">
+        <v>10187</v>
+      </c>
+      <c r="X184">
+        <v>5338</v>
+      </c>
+    </row>
+    <row r="185" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U185">
+        <v>8192</v>
+      </c>
+      <c r="V185">
+        <v>22922</v>
+      </c>
+      <c r="W185">
+        <v>20379</v>
+      </c>
+      <c r="X185">
+        <v>10712</v>
+      </c>
+    </row>
+    <row r="186" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U186" s="1">
+        <v>16384</v>
+      </c>
+      <c r="V186">
+        <v>45833</v>
+      </c>
+      <c r="W186">
+        <v>40716</v>
+      </c>
+      <c r="X186">
+        <v>21090</v>
+      </c>
+    </row>
+    <row r="187" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U187" s="1">
+        <v>32768</v>
+      </c>
+      <c r="V187">
+        <v>91785</v>
+      </c>
+      <c r="W187">
+        <v>81612</v>
+      </c>
+      <c r="X187">
+        <v>42211</v>
+      </c>
+    </row>
+    <row r="188" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U188" s="1">
+        <v>65536</v>
+      </c>
+      <c r="V188">
+        <v>184051</v>
+      </c>
+      <c r="W188">
+        <v>163207</v>
+      </c>
+      <c r="X188">
+        <v>86042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update README and measurements
</commit_message>
<xml_diff>
--- a/measurements/container-measurements.xlsx
+++ b/measurements/container-measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhultonharrop/Documents/Projects/map-vector/measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432EDA0C-4F11-AD41-A374-780453BD1DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D97FCBD-4822-6841-B4BC-744B05664741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="740" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
   </bookViews>
@@ -8857,7 +8857,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>iteration performance</a:t>
+              <a:t>iteration performance (4096 byte element)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -9739,6 +9739,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>element count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9801,6 +9856,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (ns)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -14853,7 +14968,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> performance</a:t>
+              <a:t> performance (128 byte element)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -15736,6 +15851,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>element</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -15798,6 +15972,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (ns)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -17060,7 +17294,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>iteration performance</a:t>
+              <a:t>iteration performance (32 byte element)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -17942,6 +18176,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>element count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -18004,6 +18293,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (ns)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -18042,6 +18391,685 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="403065023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>iteration performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> (4096 byte element)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>packed-hashtable values</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$89:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$E$89:$E$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>952</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1902</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10665</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23817</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50760</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99139</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>193537</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FD03-7C4F-87C1-59F5C5D821DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>absl::flat_hash_map</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$89:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$G$89:$G$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1126</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2148</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4628</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9057</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22747</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>58026</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>130152</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>279714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-FD03-7C4F-87C1-59F5C5D821DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>robin_hood::unordered_flat_map</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Performance!$B$89:$B$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="#,##0">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="#,##0">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Performance!$H$89:$H$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>62.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>681</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1362</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2693</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5689</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10842</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45659</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>228555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-FD03-7C4F-87C1-59F5C5D821DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="992529071"/>
+        <c:axId val="1031730959"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="992529071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1031730959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1031730959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="992529071"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18840,7 +19868,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$G$154</c:f>
+              <c:f>Memory!$F$156</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -18875,7 +19903,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$E$155:$E$166</c:f>
+              <c:f>Memory!$E$157:$E$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -18920,7 +19948,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$G$155:$G$166</c:f>
+              <c:f>Memory!$F$157:$F$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -18975,7 +20003,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Memory!$H$154</c:f>
+              <c:f>Memory!$G$156</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -19010,7 +20038,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Memory!$E$155:$E$166</c:f>
+              <c:f>Memory!$E$157:$E$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -19055,7 +20083,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Memory!$H$155:$H$166</c:f>
+              <c:f>Memory!$G$157:$G$168</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -25603,6 +26631,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors27.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -35687,6 +36755,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style27.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -39346,9 +40930,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>256702</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>94574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39411,16 +40995,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>300342</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>187393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1242979</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>85792</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39849,13 +41433,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>52918</xdr:colOff>
+      <xdr:colOff>52919</xdr:colOff>
       <xdr:row>132</xdr:row>
       <xdr:rowOff>86784</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>516467</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>270933</xdr:colOff>
       <xdr:row>145</xdr:row>
       <xdr:rowOff>188384</xdr:rowOff>
     </xdr:to>
@@ -39957,15 +41541,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>91015</xdr:colOff>
+      <xdr:colOff>40216</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>116738</xdr:rowOff>
+      <xdr:rowOff>32072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>155029</xdr:rowOff>
+      <xdr:colOff>474133</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -40137,15 +41721,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>124883</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>77151</xdr:rowOff>
+      <xdr:colOff>102021</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>423333</xdr:colOff>
+      <xdr:colOff>440266</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>138439</xdr:rowOff>
+      <xdr:rowOff>37468</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -40173,15 +41757,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>112183</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>67733</xdr:rowOff>
+      <xdr:colOff>146049</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>442938</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>84666</xdr:rowOff>
+      <xdr:colOff>476804</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>186267</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -40209,15 +41793,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>129117</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>80432</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
+      <xdr:colOff>464029</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>24779</xdr:rowOff>
+      <xdr:rowOff>33868</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -40237,6 +41821,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>722490</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>112889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>448394</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>115711</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C135AEE3-34D4-F01F-12A7-A2FDAACEB248}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -40542,10 +42162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD4748D-2C7E-9A48-826D-471EC314D44C}">
-  <dimension ref="C3:S166"/>
+  <dimension ref="C3:S168"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView topLeftCell="A134" zoomScale="94" workbookViewId="0">
+      <selection activeCell="L155" sqref="L155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46441,149 +48061,146 @@
         <v>6.7114093959731542E-3</v>
       </c>
     </row>
-    <row r="154" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E154" t="s">
+    <row r="156" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E156" t="s">
         <v>2</v>
       </c>
-      <c r="G154" t="s">
+      <c r="F156" t="s">
         <v>30</v>
       </c>
-      <c r="H154" t="s">
+      <c r="G156" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E155">
+    <row r="157" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E157">
         <v>32</v>
       </c>
-      <c r="G155">
+      <c r="F157">
         <v>6.04</v>
       </c>
-      <c r="H155">
+      <c r="G157">
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E156">
+    <row r="158" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E158">
         <v>64</v>
       </c>
-      <c r="G156">
+      <c r="F158">
         <v>11</v>
       </c>
-      <c r="H156">
+      <c r="G158">
         <v>35.4</v>
       </c>
     </row>
-    <row r="157" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E157">
+    <row r="159" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E159">
         <v>128</v>
       </c>
-      <c r="G157">
+      <c r="F159">
         <v>21.1</v>
       </c>
-      <c r="H157">
+      <c r="G159">
         <v>70.599999999999994</v>
       </c>
     </row>
-    <row r="158" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E158">
+    <row r="160" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E160">
         <v>256</v>
       </c>
-      <c r="G158">
+      <c r="F160">
         <v>53.4</v>
       </c>
-      <c r="H158">
+      <c r="G160">
         <v>151</v>
       </c>
     </row>
-    <row r="159" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E159">
+    <row r="161" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E161">
         <v>512</v>
       </c>
-      <c r="G159">
+      <c r="F161">
         <v>91.1</v>
       </c>
-      <c r="H159">
+      <c r="G161">
         <v>296</v>
       </c>
     </row>
-    <row r="160" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E160">
+    <row r="162" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E162">
         <v>1024</v>
       </c>
-      <c r="G160">
+      <c r="F162">
         <v>172</v>
       </c>
-      <c r="H160">
+      <c r="G162">
         <v>584</v>
       </c>
     </row>
-    <row r="161" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E161">
+    <row r="163" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E163">
         <v>2048</v>
       </c>
-      <c r="G161">
+      <c r="F163">
         <v>335</v>
       </c>
-      <c r="H161">
+      <c r="G163">
         <v>4176</v>
       </c>
     </row>
-    <row r="162" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E162">
+    <row r="164" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E164">
         <v>4096</v>
       </c>
-      <c r="G162">
+      <c r="F164">
         <v>655</v>
       </c>
-      <c r="H162">
+      <c r="G164">
         <v>8171</v>
       </c>
     </row>
-    <row r="163" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E163">
+    <row r="165" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E165">
         <v>8192</v>
       </c>
-      <c r="G163">
+      <c r="F165">
         <v>1756</v>
       </c>
-      <c r="H163">
+      <c r="G165">
         <v>16858</v>
       </c>
     </row>
-    <row r="164" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E164" s="1">
+    <row r="166" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E166" s="1">
         <v>16384</v>
       </c>
-      <c r="F164" s="1"/>
-      <c r="G164">
+      <c r="F166">
         <v>3882</v>
       </c>
-      <c r="H164">
+      <c r="G166">
         <v>35970</v>
       </c>
     </row>
-    <row r="165" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E165" s="1">
+    <row r="167" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E167" s="1">
         <v>32768</v>
       </c>
-      <c r="F165" s="1"/>
-      <c r="G165">
+      <c r="F167">
         <v>7748</v>
       </c>
-      <c r="H165">
+      <c r="G167">
         <v>72838</v>
       </c>
     </row>
-    <row r="166" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E166" s="1">
+    <row r="168" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E168" s="1">
         <v>65536</v>
       </c>
-      <c r="F166" s="1"/>
-      <c r="G166">
+      <c r="F168">
         <v>15508</v>
       </c>
-      <c r="H166">
+      <c r="G168">
         <v>161281</v>
       </c>
     </row>
@@ -46597,8 +48214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37D38E-5F04-4043-B2C6-9B4BB7553281}">
   <dimension ref="A4:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="J73" zoomScale="90" workbookViewId="0">
+      <selection activeCell="S70" sqref="S70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49316,19 +50933,19 @@
         <v>1.9811320754716981</v>
       </c>
       <c r="G103">
-        <f>I53</f>
+        <f t="shared" ref="G103:G114" si="7">I53</f>
         <v>1.9811320754716981</v>
       </c>
       <c r="H103">
-        <f>I65</f>
+        <f t="shared" ref="H103:H114" si="8">I65</f>
         <v>2.1809523809523808</v>
       </c>
       <c r="I103">
-        <f>I77</f>
+        <f t="shared" ref="I103:I114" si="9">I77</f>
         <v>2.1698113207547172</v>
       </c>
       <c r="J103">
-        <f>I89</f>
+        <f t="shared" ref="J103:J114" si="10">I89</f>
         <v>1.7037037037037037</v>
       </c>
     </row>
@@ -49353,19 +50970,19 @@
         <v>2.0784313725490198</v>
       </c>
       <c r="G104">
-        <f>I54</f>
+        <f t="shared" si="7"/>
         <v>1.945054945054945</v>
       </c>
       <c r="H104">
-        <f>I66</f>
+        <f t="shared" si="8"/>
         <v>2.6699029126213589</v>
       </c>
       <c r="I104">
-        <f>I78</f>
+        <f t="shared" si="9"/>
         <v>2.1653543307086616</v>
       </c>
       <c r="J104">
-        <f>I90</f>
+        <f t="shared" si="10"/>
         <v>1.8394648829431439</v>
       </c>
     </row>
@@ -49390,19 +51007,19 @@
         <v>2.8033472803347284</v>
       </c>
       <c r="G105">
-        <f>I55</f>
+        <f t="shared" si="7"/>
         <v>2.8092243186582806</v>
       </c>
       <c r="H105">
-        <f>I67</f>
+        <f t="shared" si="8"/>
         <v>2.8125</v>
       </c>
       <c r="I105">
-        <f>I79</f>
+        <f t="shared" si="9"/>
         <v>2.31433506044905</v>
       </c>
       <c r="J105">
-        <f>I91</f>
+        <f t="shared" si="10"/>
         <v>1.1355932203389831</v>
       </c>
     </row>
@@ -49427,19 +51044,19 @@
         <v>2.9438202247191012</v>
       </c>
       <c r="G106">
-        <f>I56</f>
+        <f t="shared" si="7"/>
         <v>2.9471316085489314</v>
       </c>
       <c r="H106">
-        <f>I68</f>
+        <f t="shared" si="8"/>
         <v>1.9245283018867925</v>
       </c>
       <c r="I106">
-        <f>I80</f>
+        <f t="shared" si="9"/>
         <v>1.6477987421383649</v>
       </c>
       <c r="J106">
-        <f>I92</f>
+        <f t="shared" si="10"/>
         <v>1.2899159663865547</v>
       </c>
     </row>
@@ -49464,19 +51081,19 @@
         <v>3.0833333333333335</v>
       </c>
       <c r="G107">
-        <f>I57</f>
+        <f t="shared" si="7"/>
         <v>1.6156250000000001</v>
       </c>
       <c r="H107">
-        <f>I69</f>
+        <f t="shared" si="8"/>
         <v>8.730407523510971</v>
       </c>
       <c r="I107">
-        <f>I81</f>
+        <f t="shared" si="9"/>
         <v>8.7156249999999993</v>
       </c>
       <c r="J107">
-        <f>I93</f>
+        <f t="shared" si="10"/>
         <v>5.968220338983051</v>
       </c>
     </row>
@@ -49501,19 +51118,19 @@
         <v>1.6682692307692308</v>
       </c>
       <c r="G108">
-        <f>I58</f>
+        <f t="shared" si="7"/>
         <v>1.6462264150943395</v>
       </c>
       <c r="H108">
-        <f>I70</f>
+        <f t="shared" si="8"/>
         <v>8.7351097178683386</v>
       </c>
       <c r="I108">
-        <f>I82</f>
+        <f t="shared" si="9"/>
         <v>8.9140625</v>
       </c>
       <c r="J108">
-        <f>I94</f>
+        <f t="shared" si="10"/>
         <v>6.7058823529411766</v>
       </c>
     </row>
@@ -49538,19 +51155,19 @@
         <v>9.4163393558523172</v>
       </c>
       <c r="G109">
-        <f>I59</f>
+        <f t="shared" si="7"/>
         <v>9.7002360346184116</v>
       </c>
       <c r="H109">
-        <f>I71</f>
+        <f t="shared" si="8"/>
         <v>8.8947368421052637</v>
       </c>
       <c r="I109">
-        <f>I83</f>
+        <f t="shared" si="9"/>
         <v>9.7042471042471039</v>
       </c>
       <c r="J109">
-        <f>I95</f>
+        <f t="shared" si="10"/>
         <v>7.0194532071503684</v>
       </c>
     </row>
@@ -49575,19 +51192,19 @@
         <v>9.7047506870828428</v>
       </c>
       <c r="G110">
-        <f>I60</f>
+        <f t="shared" si="7"/>
         <v>9.4411648957103509</v>
       </c>
       <c r="H110">
-        <f>I72</f>
+        <f t="shared" si="8"/>
         <v>9.5785575048732952</v>
       </c>
       <c r="I110">
-        <f>I84</f>
+        <f t="shared" si="9"/>
         <v>8.7279338842975207</v>
       </c>
       <c r="J110">
-        <f>I96</f>
+        <f t="shared" si="10"/>
         <v>2.6241912798874822</v>
       </c>
     </row>
@@ -49612,19 +51229,19 @@
         <v>9.58955223880597</v>
       </c>
       <c r="G111">
-        <f>I61</f>
+        <f t="shared" si="7"/>
         <v>9.7214745465184311</v>
       </c>
       <c r="H111">
-        <f>I73</f>
+        <f t="shared" si="8"/>
         <v>8.2117102744097004</v>
       </c>
       <c r="I111">
-        <f>I85</f>
+        <f t="shared" si="9"/>
         <v>3.2798314840087817</v>
       </c>
       <c r="J111">
-        <f>I97</f>
+        <f t="shared" si="10"/>
         <v>2.4537515220220851</v>
       </c>
     </row>
@@ -49649,19 +51266,19 @@
         <v>9.8131450827653364</v>
       </c>
       <c r="G112">
-        <f>I62</f>
+        <f t="shared" si="7"/>
         <v>8.4152529420755009</v>
       </c>
       <c r="H112">
-        <f>I74</f>
+        <f t="shared" si="8"/>
         <v>5.1900655188176135</v>
       </c>
       <c r="I112">
-        <f>I86</f>
+        <f t="shared" si="9"/>
         <v>4.7712178104444618</v>
       </c>
       <c r="J112">
-        <f>I98</f>
+        <f t="shared" si="10"/>
         <v>4.1800039401103231</v>
       </c>
     </row>
@@ -49686,19 +51303,19 @@
         <v>10.573198627525734</v>
       </c>
       <c r="G113">
-        <f>I63</f>
+        <f t="shared" si="7"/>
         <v>10.458307597282273</v>
       </c>
       <c r="H113">
-        <f>I75</f>
+        <f t="shared" si="8"/>
         <v>21.971772157082214</v>
       </c>
       <c r="I113">
-        <f>I87</f>
+        <f t="shared" si="9"/>
         <v>20.727859602749998</v>
       </c>
       <c r="J113">
-        <f>I99</f>
+        <f t="shared" si="10"/>
         <v>17.397805101927595</v>
       </c>
     </row>
@@ -49723,19 +51340,19 @@
         <v>13.850166445553176</v>
       </c>
       <c r="G114">
-        <f>I64</f>
+        <f t="shared" si="7"/>
         <v>22.389139483951443</v>
       </c>
       <c r="H114">
-        <f>I76</f>
+        <f t="shared" si="8"/>
         <v>23.36347713266299</v>
       </c>
       <c r="I114">
-        <f>I88</f>
+        <f t="shared" si="9"/>
         <v>24.074776908137128</v>
       </c>
       <c r="J114">
-        <f>I100</f>
+        <f t="shared" si="10"/>
         <v>19.921859902757614</v>
       </c>
     </row>
@@ -49748,11 +51365,11 @@
         <v>12.103613749877583</v>
       </c>
       <c r="D116">
-        <f t="shared" ref="D116" si="7">MAX(D103:D113)</f>
+        <f t="shared" ref="D116" si="11">MAX(D103:D113)</f>
         <v>10.320610687022901</v>
       </c>
       <c r="E116">
-        <f t="shared" ref="E116" si="8">MAX(E103:E113)</f>
+        <f t="shared" ref="E116" si="12">MAX(E103:E113)</f>
         <v>13.75</v>
       </c>
       <c r="F116">
@@ -49785,15 +51402,15 @@
         <v>1.9739776951672865</v>
       </c>
       <c r="D117">
-        <f t="shared" ref="D117" si="9">MIN(D103:D113)</f>
+        <f t="shared" ref="D117" si="13">MIN(D103:D113)</f>
         <v>1.9811320754716981</v>
       </c>
       <c r="E117">
-        <f t="shared" ref="E117:L117" si="10">MIN(E103:E113)</f>
+        <f t="shared" ref="E117:F117" si="14">MIN(E103:E113)</f>
         <v>1.9811320754716981</v>
       </c>
       <c r="F117">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1.6682692307692308</v>
       </c>
       <c r="G117">

</xml_diff>

<commit_message>
update readme with memory usage graphs
</commit_message>
<xml_diff>
--- a/measurements/container-measurements.xlsx
+++ b/measurements/container-measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomhultonharrop/Documents/Projects/map-vector/measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D97FCBD-4822-6841-B4BC-744B05664741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BFD73B-CBA4-8F4F-852C-1D53BDD4FF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="740" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
+    <workbookView xWindow="420" yWindow="740" windowWidth="28040" windowHeight="17420" xr2:uid="{1D174048-E64B-3444-BA66-F7E69AF161AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory" sheetId="1" r:id="rId1"/>
@@ -2879,11 +2879,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Container</a:t>
+              <a:t>container</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Memory Usage</a:t>
+              <a:t> memory usage (4096 byte element)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -3766,6 +3766,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>element</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> count</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3828,6 +3888,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> usage (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -20386,7 +20506,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Container Memory Usage</a:t>
+              <a:t>container memory usage (32 byte element)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -21268,6 +21388,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>element count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -21330,6 +21505,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>memory usage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -22592,7 +22827,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Container Memory Usage</a:t>
+              <a:t>container memory usage (128 byte element)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -23474,6 +23709,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>element</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -23536,6 +23830,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> usage (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -41032,15 +41386,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>656346</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>39586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>266106</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>135107</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -41104,15 +41458,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>634189</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>22832</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>226818</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>108085</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -41284,15 +41638,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:colOff>299126</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>24455</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>780817</xdr:colOff>
       <xdr:row>121</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>148618</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -42164,8 +42518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD4748D-2C7E-9A48-826D-471EC314D44C}">
   <dimension ref="C3:S168"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" zoomScale="94" workbookViewId="0">
-      <selection activeCell="L155" sqref="L155"/>
+    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -48214,7 +48568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA37D38E-5F04-4043-B2C6-9B4BB7553281}">
   <dimension ref="A4:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J73" zoomScale="90" workbookViewId="0">
+    <sheetView topLeftCell="A78" zoomScale="90" workbookViewId="0">
       <selection activeCell="S70" sqref="S70"/>
     </sheetView>
   </sheetViews>

</xml_diff>